<commit_message>
Work on dynamic addition of coefficients
</commit_message>
<xml_diff>
--- a/Proyecto.xlsx
+++ b/Proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soraya Maqueda\Desktop\Education\Spring2022\MR2007 - Control Computarizado\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACFBFAF-EFC0-4F53-AEA6-72E2DDED544D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D295213A-3E0F-490F-BB99-8FC5CB698DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{659C412E-9257-4F81-8F1D-5F8646B63D92}"/>
   </bookViews>
@@ -788,6 +788,7 @@
         <c:axId val="1333352736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1394,6 +1395,7 @@
         <c:axId val="1637845632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -4049,7 +4051,7 @@
   <dimension ref="A1:S57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Conditional showing of plot
</commit_message>
<xml_diff>
--- a/Proyecto.xlsx
+++ b/Proyecto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soraya Maqueda\Desktop\Education\Spring2022\MR2007 - Control Computarizado\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D295213A-3E0F-490F-BB99-8FC5CB698DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD08199-C9CC-4924-BD55-B077E93D6172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{659C412E-9257-4F81-8F1D-5F8646B63D92}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>k</t>
   </si>
@@ -136,12 +136,18 @@
   <si>
     <t>y2(k)</t>
   </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +194,13 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Rockwell"/>
+      <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Rockwell"/>
       <family val="1"/>
       <scheme val="minor"/>
@@ -249,7 +262,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -272,11 +285,273 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -310,22 +585,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -334,7 +594,82 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -409,7 +744,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$1</c:f>
+              <c:f>Sheet1!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -444,161 +779,155 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$7:$O$57</c:f>
+              <c:f>Sheet1!$R$10:$R$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="51"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>27</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>28</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>29</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>30</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>31</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>32</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>33</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>34</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>35</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>36</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>37</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>38</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>39</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>40</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>43</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>44</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>45</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>46</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>47</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="50">
                   <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
@@ -606,162 +935,156 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$7:$Q$57</c:f>
+              <c:f>Sheet1!$T$10:$T$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="51"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>4.3079999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75</c:v>
+                  <c:v>5.6963999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.875</c:v>
+                  <c:v>6.8821199999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9375</c:v>
+                  <c:v>7.8681960000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.96875</c:v>
+                  <c:v>8.6758068000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.984375</c:v>
+                  <c:v>9.3312704400000008</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.9921875</c:v>
+                  <c:v>9.8603288520000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.99609375</c:v>
+                  <c:v>10.285919331599999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.998046875</c:v>
+                  <c:v>10.627563590279998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.9990234375</c:v>
+                  <c:v>10.901464934723997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.99951171875</c:v>
+                  <c:v>11.120878979029197</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.999755859375</c:v>
+                  <c:v>11.296556698848356</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.9998779296875</c:v>
+                  <c:v>11.437172116891183</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.99993896484375</c:v>
+                  <c:v>11.549701072419195</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.999969482421875</c:v>
+                  <c:v>11.639742547388479</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.9999847412109375</c:v>
+                  <c:v>11.711784882637346</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.99999237060546875</c:v>
+                  <c:v>11.769423328473156</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.99999618530273438</c:v>
+                  <c:v>11.815536373960164</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.99999809265136719</c:v>
+                  <c:v>11.852427954758952</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.99999904632568359</c:v>
+                  <c:v>11.881941791602571</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.9999995231628418</c:v>
+                  <c:v>11.905553147179763</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.9999997615814209</c:v>
+                  <c:v>11.924442374692664</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.99999988079071045</c:v>
+                  <c:v>11.939553828228556</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.99999994039535522</c:v>
+                  <c:v>11.951643026820058</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.99999997019767761</c:v>
+                  <c:v>11.961314403574651</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.99999998509883881</c:v>
+                  <c:v>11.969051513919023</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.9999999925494194</c:v>
+                  <c:v>11.975241206664869</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.9999999962747097</c:v>
+                  <c:v>11.980192963096719</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.99999999813735485</c:v>
+                  <c:v>11.984154369359789</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.99999999906867743</c:v>
+                  <c:v>11.987323494929036</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.99999999953433871</c:v>
+                  <c:v>11.989858795663832</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.99999999976716936</c:v>
+                  <c:v>11.991887036391367</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.99999999988358468</c:v>
+                  <c:v>11.993509629043244</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.99999999994179234</c:v>
+                  <c:v>11.994807703199671</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.99999999997089617</c:v>
+                  <c:v>11.995846162542275</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.99999999998544808</c:v>
+                  <c:v>11.996676930025089</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.99999999999272404</c:v>
+                  <c:v>11.997341544015704</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.99999999999636202</c:v>
+                  <c:v>11.997873235210379</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.99999999999818101</c:v>
+                  <c:v>11.998298588167211</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.99999999999909051</c:v>
+                  <c:v>11.998638870533222</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.99999999999954525</c:v>
+                  <c:v>11.998911096426305</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.99999999999977263</c:v>
+                  <c:v>11.999128877140908</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.99999999999988631</c:v>
+                  <c:v>11.999303101712657</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.99999999999994316</c:v>
+                  <c:v>11.999442481370091</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.99999999999997158</c:v>
+                  <c:v>11.999553985096055</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.99999999999998579</c:v>
+                  <c:v>11.999643188076835</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.99999999999999289</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.99999999999999645</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.99999999999999822</c:v>
+                  <c:v>11.999714550461462</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1016,7 +1339,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$1</c:f>
+              <c:f>Sheet1!$V$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1051,7 +1374,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$7:$O$57</c:f>
+              <c:f>Sheet1!$R$8:$R$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -1213,7 +1536,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$S$7:$S$57</c:f>
+              <c:f>Sheet1!$V$8:$V$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -2622,9 +2945,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2743,13 +3066,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2831,14 +3154,14 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>557212</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3164904" cy="166264"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -2880,6 +3203,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3204,7 +3528,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -3269,15 +3593,15 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>1390651</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3346,14 +3670,14 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>681037</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="709233" cy="166264"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -3441,7 +3765,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -3530,14 +3854,14 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>52387</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="675057" cy="166264"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -3584,6 +3908,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3647,7 +3972,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -3719,13 +4044,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>166007</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>13606</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3753,15 +4078,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>673552</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>2722</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>13606</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>40821</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4048,107 +4373,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BFE0C0-539D-4A11-876B-93C3EB737B5D}">
-  <dimension ref="A1:S57"/>
+  <dimension ref="A1:V58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="1"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="4"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="4"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="4"/>
-      <c r="O1" s="13" t="s">
+      <c r="K1" s="1"/>
+      <c r="L1" s="4"/>
+      <c r="P1" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="S1" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="T1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="U1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="17" t="s">
+      <c r="V1" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4"/>
+    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="O2" s="9">
-        <v>-5</v>
-      </c>
-      <c r="P2" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="9">
-        <v>0</v>
-      </c>
-      <c r="R2" s="9">
-        <v>0</v>
-      </c>
-      <c r="S2" s="9">
-        <v>0</v>
-      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="4"/>
+      <c r="P2" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="28"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="39"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="O3" s="9">
-        <v>-4</v>
-      </c>
-      <c r="P3" s="9">
+      <c r="L3" s="4"/>
+      <c r="P3" s="33">
+        <f>R3-1</f>
+        <v>-6</v>
+      </c>
+      <c r="Q3" s="30">
+        <f>R3-1-$E$11</f>
+        <v>-6</v>
+      </c>
+      <c r="R3" s="21">
+        <v>-5</v>
+      </c>
+      <c r="S3" s="34">
         <v>0</v>
       </c>
-      <c r="Q3" s="9">
+      <c r="T3" s="35">
         <v>0</v>
       </c>
-      <c r="R3" s="9">
+      <c r="U3" s="34">
         <v>0</v>
       </c>
-      <c r="S3" s="9">
+      <c r="V3" s="35">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -4160,23 +4496,32 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="O4" s="9">
-        <v>-3</v>
-      </c>
-      <c r="P4" s="9">
+      <c r="L4" s="4"/>
+      <c r="P4" s="33">
+        <f t="shared" ref="P4:P58" si="0">R4-1</f>
+        <v>-5</v>
+      </c>
+      <c r="Q4" s="30">
+        <f t="shared" ref="Q4:Q58" si="1">R4-1-$E$11</f>
+        <v>-5</v>
+      </c>
+      <c r="R4" s="21">
+        <v>-4</v>
+      </c>
+      <c r="S4" s="16">
         <v>0</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="T4" s="17">
         <v>0</v>
       </c>
-      <c r="R4" s="9">
+      <c r="U4" s="16">
         <v>0</v>
       </c>
-      <c r="S4" s="9">
+      <c r="V4" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -4188,23 +4533,32 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="O5" s="9">
-        <v>-2</v>
-      </c>
-      <c r="P5" s="9">
+      <c r="L5" s="4"/>
+      <c r="P5" s="33">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="Q5" s="30">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="R5" s="21">
+        <v>-3</v>
+      </c>
+      <c r="S5" s="16">
         <v>0</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="T5" s="17">
         <v>0</v>
       </c>
-      <c r="R5" s="9">
+      <c r="U5" s="16">
         <v>0</v>
       </c>
-      <c r="S5" s="9">
+      <c r="V5" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -4216,23 +4570,32 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
-      <c r="O6" s="9">
-        <v>-1</v>
-      </c>
-      <c r="P6" s="9">
+      <c r="L6" s="4"/>
+      <c r="P6" s="33">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="Q6" s="30">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+      <c r="R6" s="21">
+        <v>-2</v>
+      </c>
+      <c r="S6" s="16">
         <v>0</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="T6" s="17">
         <v>0</v>
       </c>
-      <c r="R6" s="9">
+      <c r="U6" s="16">
         <v>0</v>
       </c>
-      <c r="S6" s="9">
+      <c r="V6" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -4241,1136 +4604,1598 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-      <c r="O7" s="9">
+      <c r="L7" s="4"/>
+      <c r="P7" s="33">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="Q7" s="30">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="R7" s="21">
+        <v>-1</v>
+      </c>
+      <c r="S7" s="16">
         <v>0</v>
       </c>
-      <c r="P7" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="9">
+      <c r="T7" s="17">
         <v>0</v>
       </c>
-      <c r="R7" s="9">
-        <v>1</v>
-      </c>
-      <c r="S7" s="9">
+      <c r="U7" s="16">
         <v>0</v>
       </c>
+      <c r="V7" s="17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="6"/>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="11"/>
-      <c r="O8" s="9">
-        <v>1</v>
-      </c>
-      <c r="P8" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="9">
+      <c r="I8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="P8" s="33">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="Q8" s="30">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="R8" s="21">
         <v>0</v>
       </c>
-      <c r="R8" s="9">
-        <v>1</v>
-      </c>
-      <c r="S8" s="9">
+      <c r="S8" s="16">
+        <v>1</v>
+      </c>
+      <c r="T8" s="17">
         <v>0</v>
       </c>
+      <c r="U8" s="16">
+        <v>1</v>
+      </c>
+      <c r="V8" s="17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+    <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="9">
-        <v>1</v>
-      </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="11"/>
-      <c r="O9" s="9">
+      <c r="I9" s="4"/>
+      <c r="J9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="15"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="11"/>
+      <c r="P9" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="21">
+        <v>1</v>
+      </c>
+      <c r="S9" s="16">
+        <v>1</v>
+      </c>
+      <c r="T9" s="17">
+        <f>($A$11*T8)+($B$11*T7)+($C$11*S8)+($D$11*S7)</f>
+        <v>0</v>
+      </c>
+      <c r="U9" s="16">
+        <v>1</v>
+      </c>
+      <c r="V9" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="P9" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="9">
-        <f>($A$10*Q8)+($B$10*P9)+($C$10*P8)</f>
-        <v>0.5</v>
-      </c>
-      <c r="R9" s="9">
-        <v>1</v>
-      </c>
-      <c r="S9" s="9">
-        <f>($I$16*S8)+($K$16*R6)+($L$16*R5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="B10" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="C10" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="D10" s="10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4"/>
+      <c r="B10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>5</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="9">
-        <v>3.34</v>
-      </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="11"/>
-      <c r="O10" s="9">
-        <v>3</v>
-      </c>
-      <c r="P10" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="9">
-        <f t="shared" ref="Q10:Q57" si="0">($A$10*Q9)+($B$10*P10)+($C$10*P9)</f>
-        <v>0.75</v>
-      </c>
-      <c r="R10" s="9">
-        <v>1</v>
-      </c>
-      <c r="S10" s="9">
-        <f>($I$16*S9)+($K$16*R7)+($L$16*R6)</f>
-        <v>0.25873804275132251</v>
+      <c r="I10" s="4"/>
+      <c r="J10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="9">
+        <v>1</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10" s="11"/>
+      <c r="P10" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q10" s="30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R10" s="21">
+        <v>2</v>
+      </c>
+      <c r="S10" s="16">
+        <v>1</v>
+      </c>
+      <c r="T10" s="17">
+        <f t="shared" ref="T10:T58" si="2">($A$11*T9)+($B$11*T8)+($C$11*S9)+($D$11*S8)</f>
+        <v>1.2</v>
+      </c>
+      <c r="U10" s="16">
+        <v>1</v>
+      </c>
+      <c r="V10" s="17">
+        <f t="shared" ref="V10:V41" si="3">($J$17*V9)+($L$17*U7)+($M$17*U6)</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+    <row r="11" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>1.3</v>
+      </c>
+      <c r="B11" s="9">
+        <v>-0.4</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
+        <v>1.2</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0</v>
+      </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="9">
-        <v>1.46</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="O11" s="9">
-        <v>4</v>
-      </c>
-      <c r="P11" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="9">
+      <c r="I11" s="4"/>
+      <c r="J11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="9">
+        <v>3.34</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="M11" s="11"/>
+      <c r="P11" s="33">
         <f t="shared" si="0"/>
-        <v>0.875</v>
-      </c>
-      <c r="R11" s="9">
-        <v>1</v>
-      </c>
-      <c r="S11" s="9">
-        <f>($I$16*S10)+($K$16*R8)+($L$16*R7)</f>
-        <v>1.1505307107358598</v>
+        <v>2</v>
+      </c>
+      <c r="Q11" s="30">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="R11" s="21">
+        <v>3</v>
+      </c>
+      <c r="S11" s="16">
+        <v>1</v>
+      </c>
+      <c r="T11" s="17">
+        <f t="shared" si="2"/>
+        <v>2.76</v>
+      </c>
+      <c r="U11" s="16">
+        <v>1</v>
+      </c>
+      <c r="V11" s="17">
+        <f t="shared" si="3"/>
+        <v>0.25873804275132251</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="9">
-        <v>1</v>
+      <c r="I12" s="4"/>
+      <c r="J12" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="K12" s="9">
-        <f>J11-(J12*M16)</f>
-        <v>0.45999999999999996</v>
-      </c>
-      <c r="L12" s="9">
-        <f>1-(K12/J12)</f>
-        <v>0.54</v>
-      </c>
-      <c r="O12" s="9">
-        <v>5</v>
-      </c>
-      <c r="P12" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="9">
+        <v>1.46</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P12" s="33">
         <f t="shared" si="0"/>
-        <v>0.9375</v>
-      </c>
-      <c r="R12" s="9">
-        <v>1</v>
-      </c>
-      <c r="S12" s="9">
-        <f>($I$16*S11)+($K$16*R9)+($L$16*R8)</f>
-        <v>1.8115826892660978</v>
+        <v>3</v>
+      </c>
+      <c r="Q12" s="30">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="R12" s="21">
+        <v>4</v>
+      </c>
+      <c r="S12" s="16">
+        <v>1</v>
+      </c>
+      <c r="T12" s="17">
+        <f t="shared" si="2"/>
+        <v>4.3079999999999998</v>
+      </c>
+      <c r="U12" s="16">
+        <v>1</v>
+      </c>
+      <c r="V12" s="17">
+        <f t="shared" si="3"/>
+        <v>1.1505307107358598</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="F13" s="4"/>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="O13" s="9">
-        <v>6</v>
-      </c>
-      <c r="P13" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="9">
+      <c r="J13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="9">
+        <v>1</v>
+      </c>
+      <c r="L13" s="9">
+        <f>K12-(K13*N17)</f>
+        <v>0.45999999999999996</v>
+      </c>
+      <c r="M13" s="9">
+        <f>1-(L13/K13)</f>
+        <v>0.54</v>
+      </c>
+      <c r="P13" s="33">
         <f t="shared" si="0"/>
-        <v>0.96875</v>
-      </c>
-      <c r="R13" s="9">
-        <v>1</v>
-      </c>
-      <c r="S13" s="9">
-        <f>($I$16*S12)+($K$16*R10)+($L$16*R9)</f>
-        <v>2.3015953727145329</v>
+        <v>4</v>
+      </c>
+      <c r="Q13" s="30">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="R13" s="21">
+        <v>5</v>
+      </c>
+      <c r="S13" s="16">
+        <v>1</v>
+      </c>
+      <c r="T13" s="17">
+        <f t="shared" si="2"/>
+        <v>5.6963999999999997</v>
+      </c>
+      <c r="U13" s="16">
+        <v>1</v>
+      </c>
+      <c r="V13" s="17">
+        <f t="shared" si="3"/>
+        <v>1.8115826892660978</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.2">
-      <c r="F14" s="4"/>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="21" t="s">
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="P14" s="33">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="Q14" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="R14" s="21">
         <v>6</v>
       </c>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="9">
-        <v>7</v>
-      </c>
-      <c r="P14" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="9">
-        <f t="shared" si="0"/>
-        <v>0.984375</v>
-      </c>
-      <c r="R14" s="9">
-        <v>1</v>
-      </c>
-      <c r="S14" s="9">
-        <f>($I$16*S13)+($K$16*R11)+($L$16*R10)</f>
-        <v>2.6648231335241963</v>
+      <c r="S14" s="16">
+        <v>1</v>
+      </c>
+      <c r="T14" s="17">
+        <f t="shared" si="2"/>
+        <v>6.8821199999999996</v>
+      </c>
+      <c r="U14" s="16">
+        <v>1</v>
+      </c>
+      <c r="V14" s="17">
+        <f t="shared" si="3"/>
+        <v>2.3015953727145329</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+    <row r="15" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="4"/>
+      <c r="J15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="33">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="Q15" s="30">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="R15" s="21">
+        <v>7</v>
+      </c>
+      <c r="S15" s="16">
+        <v>1</v>
+      </c>
+      <c r="T15" s="17">
+        <f t="shared" si="2"/>
+        <v>7.8681960000000002</v>
+      </c>
+      <c r="U15" s="16">
+        <v>1</v>
+      </c>
+      <c r="V15" s="17">
+        <f t="shared" si="3"/>
+        <v>2.6648231335241963</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="K16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="L16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="M16" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="10" t="s">
+      <c r="N16" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N15" s="8"/>
-      <c r="O15" s="9">
+      <c r="O16" s="8"/>
+      <c r="P16" s="33">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="Q16" s="30">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="R16" s="21">
         <v>8</v>
       </c>
-      <c r="P15" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="9">
+      <c r="S16" s="16">
+        <v>1</v>
+      </c>
+      <c r="T16" s="17">
+        <f t="shared" si="2"/>
+        <v>8.6758068000000002</v>
+      </c>
+      <c r="U16" s="16">
+        <v>1</v>
+      </c>
+      <c r="V16" s="17">
+        <f t="shared" si="3"/>
+        <v>2.9340700544290224</v>
+      </c>
+    </row>
+    <row r="17" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="J17" s="9">
+        <f>EXP(1)^(-K13/K11)</f>
+        <v>0.74126195724867749</v>
+      </c>
+      <c r="K17" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="L17" s="9">
+        <f>K10*(1-J17)</f>
+        <v>0.25873804275132251</v>
+      </c>
+      <c r="M17" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="N17" s="10">
+        <v>1</v>
+      </c>
+      <c r="O17" s="8"/>
+      <c r="P17" s="33">
         <f t="shared" si="0"/>
-        <v>0.9921875</v>
-      </c>
-      <c r="R15" s="9">
-        <v>1</v>
-      </c>
-      <c r="S15" s="9">
-        <f>($I$16*S14)+($K$16*R12)+($L$16*R11)</f>
-        <v>2.9340700544290224</v>
+        <v>8</v>
+      </c>
+      <c r="Q17" s="30">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="R17" s="21">
+        <v>9</v>
+      </c>
+      <c r="S17" s="16">
+        <v>1</v>
+      </c>
+      <c r="T17" s="17">
+        <f t="shared" si="2"/>
+        <v>9.3312704400000008</v>
+      </c>
+      <c r="U17" s="16">
+        <v>1</v>
+      </c>
+      <c r="V17" s="17">
+        <f t="shared" si="3"/>
+        <v>3.1336525540021132</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="I16" s="9">
-        <f>EXP(1)^(-J12/J10)</f>
-        <v>0.74126195724867749</v>
-      </c>
-      <c r="J16" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K16" s="9">
-        <f>J9*(1-I16)</f>
-        <v>0.25873804275132251</v>
-      </c>
-      <c r="L16" s="10">
-        <v>0.7</v>
-      </c>
-      <c r="M16" s="10">
-        <v>1</v>
-      </c>
-      <c r="N16" s="8"/>
-      <c r="O16" s="9">
+    <row r="18" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="P18" s="33">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="P16" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="9">
+      <c r="Q18" s="30">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="R18" s="21">
+        <v>10</v>
+      </c>
+      <c r="S18" s="16">
+        <v>1</v>
+      </c>
+      <c r="T18" s="17">
+        <f t="shared" si="2"/>
+        <v>9.8603288520000003</v>
+      </c>
+      <c r="U18" s="16">
+        <v>1</v>
+      </c>
+      <c r="V18" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2815954682682458</v>
+      </c>
+    </row>
+    <row r="19" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="P19" s="33">
         <f t="shared" si="0"/>
-        <v>0.99609375</v>
-      </c>
-      <c r="R16" s="9">
-        <v>1</v>
-      </c>
-      <c r="S16" s="9">
-        <f>($I$16*S15)+($K$16*R13)+($L$16*R12)</f>
-        <v>3.1336525540021132</v>
+        <v>10</v>
+      </c>
+      <c r="Q19" s="30">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="R19" s="21">
+        <v>11</v>
+      </c>
+      <c r="S19" s="16">
+        <v>1</v>
+      </c>
+      <c r="T19" s="17">
+        <f t="shared" si="2"/>
+        <v>10.285919331599999</v>
+      </c>
+      <c r="U19" s="16">
+        <v>1</v>
+      </c>
+      <c r="V19" s="17">
+        <f t="shared" si="3"/>
+        <v>3.3912599224582332</v>
       </c>
     </row>
-    <row r="17" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O17" s="9">
-        <v>10</v>
-      </c>
-      <c r="P17" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="9">
+    <row r="20" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="P20" s="33">
         <f t="shared" si="0"/>
-        <v>0.998046875</v>
-      </c>
-      <c r="R17" s="9">
-        <v>1</v>
-      </c>
-      <c r="S17" s="9">
-        <f>($I$16*S16)+($K$16*R14)+($L$16*R13)</f>
-        <v>3.2815954682682458</v>
+        <v>11</v>
+      </c>
+      <c r="Q20" s="30">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="R20" s="21">
+        <v>12</v>
+      </c>
+      <c r="S20" s="16">
+        <v>1</v>
+      </c>
+      <c r="T20" s="17">
+        <f t="shared" si="2"/>
+        <v>10.627563590279998</v>
+      </c>
+      <c r="U20" s="16">
+        <v>1</v>
+      </c>
+      <c r="V20" s="17">
+        <f t="shared" si="3"/>
+        <v>3.4725500104117106</v>
       </c>
     </row>
-    <row r="18" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O18" s="9">
-        <v>11</v>
-      </c>
-      <c r="P18" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="9">
+    <row r="21" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="P21" s="33">
         <f t="shared" si="0"/>
-        <v>0.9990234375</v>
-      </c>
-      <c r="R18" s="9">
-        <v>1</v>
-      </c>
-      <c r="S18" s="9">
-        <f>($I$16*S17)+($K$16*R15)+($L$16*R14)</f>
-        <v>3.3912599224582332</v>
+        <v>12</v>
+      </c>
+      <c r="Q21" s="30">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="R21" s="21">
+        <v>13</v>
+      </c>
+      <c r="S21" s="16">
+        <v>1</v>
+      </c>
+      <c r="T21" s="17">
+        <f t="shared" si="2"/>
+        <v>10.901464934723997</v>
+      </c>
+      <c r="U21" s="16">
+        <v>1</v>
+      </c>
+      <c r="V21" s="17">
+        <f t="shared" si="3"/>
+        <v>3.5328072601130227</v>
       </c>
     </row>
-    <row r="19" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O19" s="9">
-        <v>12</v>
-      </c>
-      <c r="P19" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="9">
+    <row r="22" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="P22" s="33">
         <f t="shared" si="0"/>
-        <v>0.99951171875</v>
-      </c>
-      <c r="R19" s="9">
-        <v>1</v>
-      </c>
-      <c r="S19" s="9">
-        <f>($I$16*S18)+($K$16*R16)+($L$16*R15)</f>
-        <v>3.4725500104117106</v>
+        <v>13</v>
+      </c>
+      <c r="Q22" s="30">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="R22" s="21">
+        <v>14</v>
+      </c>
+      <c r="S22" s="16">
+        <v>1</v>
+      </c>
+      <c r="T22" s="17">
+        <f t="shared" si="2"/>
+        <v>11.120878979029197</v>
+      </c>
+      <c r="U22" s="16">
+        <v>1</v>
+      </c>
+      <c r="V22" s="17">
+        <f t="shared" si="3"/>
+        <v>3.5774736669650391</v>
       </c>
     </row>
-    <row r="20" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O20" s="9">
-        <v>13</v>
-      </c>
-      <c r="P20" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="9">
+    <row r="23" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="P23" s="33">
         <f t="shared" si="0"/>
-        <v>0.999755859375</v>
-      </c>
-      <c r="R20" s="9">
-        <v>1</v>
-      </c>
-      <c r="S20" s="9">
-        <f>($I$16*S19)+($K$16*R17)+($L$16*R16)</f>
-        <v>3.5328072601130227</v>
+        <v>14</v>
+      </c>
+      <c r="Q23" s="30">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="R23" s="21">
+        <v>15</v>
+      </c>
+      <c r="S23" s="16">
+        <v>1</v>
+      </c>
+      <c r="T23" s="17">
+        <f t="shared" si="2"/>
+        <v>11.296556698848356</v>
+      </c>
+      <c r="U23" s="16">
+        <v>1</v>
+      </c>
+      <c r="V23" s="17">
+        <f t="shared" si="3"/>
+        <v>3.6105831751314312</v>
       </c>
     </row>
-    <row r="21" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O21" s="9">
-        <v>14</v>
-      </c>
-      <c r="P21" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="9">
+    <row r="24" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="P24" s="33">
         <f t="shared" si="0"/>
-        <v>0.9998779296875</v>
-      </c>
-      <c r="R21" s="9">
-        <v>1</v>
-      </c>
-      <c r="S21" s="9">
-        <f>($I$16*S20)+($K$16*R18)+($L$16*R17)</f>
-        <v>3.5774736669650391</v>
+        <v>15</v>
+      </c>
+      <c r="Q24" s="30">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="R24" s="21">
+        <v>16</v>
+      </c>
+      <c r="S24" s="16">
+        <v>1</v>
+      </c>
+      <c r="T24" s="17">
+        <f t="shared" si="2"/>
+        <v>11.437172116891183</v>
+      </c>
+      <c r="U24" s="16">
+        <v>1</v>
+      </c>
+      <c r="V24" s="17">
+        <f t="shared" si="3"/>
+        <v>3.6351259939583915</v>
       </c>
     </row>
-    <row r="22" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O22" s="9">
-        <v>15</v>
-      </c>
-      <c r="P22" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="9">
+    <row r="25" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="P25" s="33">
         <f t="shared" si="0"/>
-        <v>0.99993896484375</v>
-      </c>
-      <c r="R22" s="9">
-        <v>1</v>
-      </c>
-      <c r="S22" s="9">
-        <f>($I$16*S21)+($K$16*R19)+($L$16*R18)</f>
-        <v>3.6105831751314312</v>
+        <v>16</v>
+      </c>
+      <c r="Q25" s="30">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="R25" s="21">
+        <v>17</v>
+      </c>
+      <c r="S25" s="16">
+        <v>1</v>
+      </c>
+      <c r="T25" s="17">
+        <f t="shared" si="2"/>
+        <v>11.549701072419195</v>
+      </c>
+      <c r="U25" s="16">
+        <v>1</v>
+      </c>
+      <c r="V25" s="17">
+        <f t="shared" si="3"/>
+        <v>3.6533186518784637</v>
       </c>
     </row>
-    <row r="23" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O23" s="9">
-        <v>16</v>
-      </c>
-      <c r="P23" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="9">
+    <row r="26" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="P26" s="33">
         <f t="shared" si="0"/>
-        <v>0.999969482421875</v>
-      </c>
-      <c r="R23" s="9">
-        <v>1</v>
-      </c>
-      <c r="S23" s="9">
-        <f>($I$16*S22)+($K$16*R20)+($L$16*R19)</f>
-        <v>3.6351259939583915</v>
+        <v>17</v>
+      </c>
+      <c r="Q26" s="30">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="R26" s="21">
+        <v>18</v>
+      </c>
+      <c r="S26" s="16">
+        <v>1</v>
+      </c>
+      <c r="T26" s="17">
+        <f t="shared" si="2"/>
+        <v>11.639742547388479</v>
+      </c>
+      <c r="U26" s="16">
+        <v>1</v>
+      </c>
+      <c r="V26" s="17">
+        <f t="shared" si="3"/>
+        <v>3.6668041770958526</v>
       </c>
     </row>
-    <row r="24" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O24" s="9">
-        <v>17</v>
-      </c>
-      <c r="P24" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q24" s="9">
+    <row r="27" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="P27" s="33">
         <f t="shared" si="0"/>
-        <v>0.9999847412109375</v>
-      </c>
-      <c r="R24" s="9">
-        <v>1</v>
-      </c>
-      <c r="S24" s="9">
-        <f>($I$16*S23)+($K$16*R21)+($L$16*R20)</f>
-        <v>3.6533186518784637</v>
+        <v>18</v>
+      </c>
+      <c r="Q27" s="30">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="R27" s="21">
+        <v>19</v>
+      </c>
+      <c r="S27" s="16">
+        <v>1</v>
+      </c>
+      <c r="T27" s="17">
+        <f t="shared" si="2"/>
+        <v>11.711784882637346</v>
+      </c>
+      <c r="U27" s="16">
+        <v>1</v>
+      </c>
+      <c r="V27" s="17">
+        <f t="shared" si="3"/>
+        <v>3.6768004839130208</v>
       </c>
     </row>
-    <row r="25" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O25" s="9">
-        <v>18</v>
-      </c>
-      <c r="P25" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="9">
+    <row r="28" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="P28" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999237060546875</v>
-      </c>
-      <c r="R25" s="9">
-        <v>1</v>
-      </c>
-      <c r="S25" s="9">
-        <f>($I$16*S24)+($K$16*R22)+($L$16*R21)</f>
-        <v>3.6668041770958526</v>
+        <v>19</v>
+      </c>
+      <c r="Q28" s="30">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="R28" s="21">
+        <v>20</v>
+      </c>
+      <c r="S28" s="16">
+        <v>1</v>
+      </c>
+      <c r="T28" s="17">
+        <f t="shared" si="2"/>
+        <v>11.769423328473156</v>
+      </c>
+      <c r="U28" s="16">
+        <v>1</v>
+      </c>
+      <c r="V28" s="17">
+        <f t="shared" si="3"/>
+        <v>3.6842103658695731</v>
       </c>
     </row>
-    <row r="26" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O26" s="9">
-        <v>19</v>
-      </c>
-      <c r="P26" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="9">
+    <row r="29" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="P29" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999618530273438</v>
-      </c>
-      <c r="R26" s="9">
-        <v>1</v>
-      </c>
-      <c r="S26" s="9">
-        <f>($I$16*S25)+($K$16*R23)+($L$16*R22)</f>
-        <v>3.6768004839130208</v>
+        <v>20</v>
+      </c>
+      <c r="Q29" s="30">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="R29" s="21">
+        <v>21</v>
+      </c>
+      <c r="S29" s="16">
+        <v>1</v>
+      </c>
+      <c r="T29" s="17">
+        <f t="shared" si="2"/>
+        <v>11.815536373960164</v>
+      </c>
+      <c r="U29" s="16">
+        <v>1</v>
+      </c>
+      <c r="V29" s="17">
+        <f t="shared" si="3"/>
+        <v>3.6897030294716684</v>
       </c>
     </row>
-    <row r="27" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O27" s="9">
-        <v>20</v>
-      </c>
-      <c r="P27" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="9">
+    <row r="30" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="P30" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999809265136719</v>
-      </c>
-      <c r="R27" s="9">
-        <v>1</v>
-      </c>
-      <c r="S27" s="9">
-        <f>($I$16*S26)+($K$16*R24)+($L$16*R23)</f>
-        <v>3.6842103658695731</v>
+        <v>21</v>
+      </c>
+      <c r="Q30" s="30">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="R30" s="21">
+        <v>22</v>
+      </c>
+      <c r="S30" s="16">
+        <v>1</v>
+      </c>
+      <c r="T30" s="17">
+        <f t="shared" si="2"/>
+        <v>11.852427954758952</v>
+      </c>
+      <c r="U30" s="16">
+        <v>1</v>
+      </c>
+      <c r="V30" s="17">
+        <f t="shared" si="3"/>
+        <v>3.6937745320438662</v>
       </c>
     </row>
-    <row r="28" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O28" s="9">
-        <v>21</v>
-      </c>
-      <c r="P28" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q28" s="9">
+    <row r="31" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="P31" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999904632568359</v>
-      </c>
-      <c r="R28" s="9">
-        <v>1</v>
-      </c>
-      <c r="S28" s="9">
-        <f>($I$16*S27)+($K$16*R25)+($L$16*R24)</f>
-        <v>3.6897030294716684</v>
+        <v>22</v>
+      </c>
+      <c r="Q31" s="30">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="R31" s="21">
+        <v>23</v>
+      </c>
+      <c r="S31" s="16">
+        <v>1</v>
+      </c>
+      <c r="T31" s="17">
+        <f t="shared" si="2"/>
+        <v>11.881941791602571</v>
+      </c>
+      <c r="U31" s="16">
+        <v>1</v>
+      </c>
+      <c r="V31" s="17">
+        <f t="shared" si="3"/>
+        <v>3.6967925820094765</v>
       </c>
     </row>
-    <row r="29" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O29" s="9">
-        <v>22</v>
-      </c>
-      <c r="P29" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q29" s="9">
+    <row r="32" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="P32" s="33">
         <f t="shared" si="0"/>
-        <v>0.9999995231628418</v>
-      </c>
-      <c r="R29" s="9">
-        <v>1</v>
-      </c>
-      <c r="S29" s="9">
-        <f>($I$16*S28)+($K$16*R26)+($L$16*R25)</f>
-        <v>3.6937745320438662</v>
+        <v>23</v>
+      </c>
+      <c r="Q32" s="30">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="R32" s="21">
+        <v>24</v>
+      </c>
+      <c r="S32" s="16">
+        <v>1</v>
+      </c>
+      <c r="T32" s="17">
+        <f t="shared" si="2"/>
+        <v>11.905553147179763</v>
+      </c>
+      <c r="U32" s="16">
+        <v>1</v>
+      </c>
+      <c r="V32" s="17">
+        <f t="shared" si="3"/>
+        <v>3.699029747634059</v>
       </c>
     </row>
-    <row r="30" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O30" s="9">
-        <v>23</v>
-      </c>
-      <c r="P30" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q30" s="9">
+    <row r="33" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P33" s="33">
         <f t="shared" si="0"/>
-        <v>0.9999997615814209</v>
-      </c>
-      <c r="R30" s="9">
-        <v>1</v>
-      </c>
-      <c r="S30" s="9">
-        <f>($I$16*S29)+($K$16*R27)+($L$16*R26)</f>
-        <v>3.6967925820094765</v>
+        <v>24</v>
+      </c>
+      <c r="Q33" s="30">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="R33" s="21">
+        <v>25</v>
+      </c>
+      <c r="S33" s="16">
+        <v>1</v>
+      </c>
+      <c r="T33" s="17">
+        <f t="shared" si="2"/>
+        <v>11.924442374692664</v>
+      </c>
+      <c r="U33" s="16">
+        <v>1</v>
+      </c>
+      <c r="V33" s="17">
+        <f t="shared" si="3"/>
+        <v>3.7006880734036267</v>
       </c>
     </row>
-    <row r="31" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O31" s="9">
-        <v>24</v>
-      </c>
-      <c r="P31" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q31" s="9">
+    <row r="34" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P34" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999988079071045</v>
-      </c>
-      <c r="R31" s="9">
-        <v>1</v>
-      </c>
-      <c r="S31" s="9">
-        <f>($I$16*S30)+($K$16*R28)+($L$16*R27)</f>
-        <v>3.699029747634059</v>
+        <v>25</v>
+      </c>
+      <c r="Q34" s="30">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="R34" s="21">
+        <v>26</v>
+      </c>
+      <c r="S34" s="16">
+        <v>1</v>
+      </c>
+      <c r="T34" s="17">
+        <f t="shared" si="2"/>
+        <v>11.939553828228556</v>
+      </c>
+      <c r="U34" s="16">
+        <v>1</v>
+      </c>
+      <c r="V34" s="17">
+        <f t="shared" si="3"/>
+        <v>3.7019173272093324</v>
       </c>
     </row>
-    <row r="32" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O32" s="9">
-        <v>25</v>
-      </c>
-      <c r="P32" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q32" s="9">
+    <row r="35" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P35" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999994039535522</v>
-      </c>
-      <c r="R32" s="9">
-        <v>1</v>
-      </c>
-      <c r="S32" s="9">
-        <f>($I$16*S31)+($K$16*R29)+($L$16*R28)</f>
-        <v>3.7006880734036267</v>
+        <v>26</v>
+      </c>
+      <c r="Q35" s="30">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="R35" s="21">
+        <v>27</v>
+      </c>
+      <c r="S35" s="16">
+        <v>1</v>
+      </c>
+      <c r="T35" s="17">
+        <f t="shared" si="2"/>
+        <v>11.951643026820058</v>
+      </c>
+      <c r="U35" s="16">
+        <v>1</v>
+      </c>
+      <c r="V35" s="17">
+        <f t="shared" si="3"/>
+        <v>3.702828526291305</v>
       </c>
     </row>
-    <row r="33" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O33" s="9">
-        <v>26</v>
-      </c>
-      <c r="P33" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q33" s="9">
+    <row r="36" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P36" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999997019767761</v>
-      </c>
-      <c r="R33" s="9">
-        <v>1</v>
-      </c>
-      <c r="S33" s="9">
-        <f>($I$16*S32)+($K$16*R30)+($L$16*R29)</f>
-        <v>3.7019173272093324</v>
+        <v>27</v>
+      </c>
+      <c r="Q36" s="30">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="R36" s="21">
+        <v>28</v>
+      </c>
+      <c r="S36" s="16">
+        <v>1</v>
+      </c>
+      <c r="T36" s="17">
+        <f t="shared" si="2"/>
+        <v>11.961314403574651</v>
+      </c>
+      <c r="U36" s="16">
+        <v>1</v>
+      </c>
+      <c r="V36" s="17">
+        <f t="shared" si="3"/>
+        <v>3.7035039635062512</v>
       </c>
     </row>
-    <row r="34" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O34" s="9">
-        <v>27</v>
-      </c>
-      <c r="P34" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="9">
+    <row r="37" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P37" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999998509883881</v>
-      </c>
-      <c r="R34" s="9">
-        <v>1</v>
-      </c>
-      <c r="S34" s="9">
-        <f>($I$16*S33)+($K$16*R31)+($L$16*R30)</f>
-        <v>3.702828526291305</v>
+        <v>28</v>
+      </c>
+      <c r="Q37" s="30">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="R37" s="21">
+        <v>29</v>
+      </c>
+      <c r="S37" s="16">
+        <v>1</v>
+      </c>
+      <c r="T37" s="17">
+        <f t="shared" si="2"/>
+        <v>11.969051513919023</v>
+      </c>
+      <c r="U37" s="16">
+        <v>1</v>
+      </c>
+      <c r="V37" s="17">
+        <f t="shared" si="3"/>
+        <v>3.7040046394182014</v>
       </c>
     </row>
-    <row r="35" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O35" s="9">
-        <v>28</v>
-      </c>
-      <c r="P35" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q35" s="9">
+    <row r="38" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P38" s="33">
         <f t="shared" si="0"/>
-        <v>0.9999999925494194</v>
-      </c>
-      <c r="R35" s="9">
-        <v>1</v>
-      </c>
-      <c r="S35" s="9">
-        <f>($I$16*S34)+($K$16*R32)+($L$16*R31)</f>
-        <v>3.7035039635062512</v>
+        <v>29</v>
+      </c>
+      <c r="Q38" s="30">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="R38" s="21">
+        <v>30</v>
+      </c>
+      <c r="S38" s="16">
+        <v>1</v>
+      </c>
+      <c r="T38" s="17">
+        <f t="shared" si="2"/>
+        <v>11.975241206664869</v>
+      </c>
+      <c r="U38" s="16">
+        <v>1</v>
+      </c>
+      <c r="V38" s="17">
+        <f t="shared" si="3"/>
+        <v>3.7043757714246404</v>
       </c>
     </row>
-    <row r="36" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O36" s="9">
-        <v>29</v>
-      </c>
-      <c r="P36" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q36" s="9">
+    <row r="39" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P39" s="33">
         <f t="shared" si="0"/>
-        <v>0.9999999962747097</v>
-      </c>
-      <c r="R36" s="9">
-        <v>1</v>
-      </c>
-      <c r="S36" s="9">
-        <f>($I$16*S35)+($K$16*R33)+($L$16*R32)</f>
-        <v>3.7040046394182014</v>
+        <v>30</v>
+      </c>
+      <c r="Q39" s="30">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="R39" s="21">
+        <v>31</v>
+      </c>
+      <c r="S39" s="16">
+        <v>1</v>
+      </c>
+      <c r="T39" s="17">
+        <f t="shared" si="2"/>
+        <v>11.980192963096719</v>
+      </c>
+      <c r="U39" s="16">
+        <v>1</v>
+      </c>
+      <c r="V39" s="17">
+        <f t="shared" si="3"/>
+        <v>3.7046508774621314</v>
       </c>
     </row>
-    <row r="37" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O37" s="9">
-        <v>30</v>
-      </c>
-      <c r="P37" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q37" s="9">
+    <row r="40" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P40" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999813735485</v>
-      </c>
-      <c r="R37" s="9">
-        <v>1</v>
-      </c>
-      <c r="S37" s="9">
-        <f>($I$16*S36)+($K$16*R34)+($L$16*R33)</f>
-        <v>3.7043757714246404</v>
+        <v>31</v>
+      </c>
+      <c r="Q40" s="30">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="R40" s="21">
+        <v>32</v>
+      </c>
+      <c r="S40" s="16">
+        <v>1</v>
+      </c>
+      <c r="T40" s="17">
+        <f t="shared" si="2"/>
+        <v>11.984154369359789</v>
+      </c>
+      <c r="U40" s="16">
+        <v>1</v>
+      </c>
+      <c r="V40" s="17">
+        <f t="shared" si="3"/>
+        <v>3.7048548031019326</v>
       </c>
     </row>
-    <row r="38" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O38" s="9">
-        <v>31</v>
-      </c>
-      <c r="P38" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q38" s="9">
+    <row r="41" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P41" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999906867743</v>
-      </c>
-      <c r="R38" s="9">
-        <v>1</v>
-      </c>
-      <c r="S38" s="9">
-        <f>($I$16*S37)+($K$16*R35)+($L$16*R34)</f>
-        <v>3.7046508774621314</v>
+        <v>32</v>
+      </c>
+      <c r="Q41" s="30">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="R41" s="21">
+        <v>33</v>
+      </c>
+      <c r="S41" s="16">
+        <v>1</v>
+      </c>
+      <c r="T41" s="17">
+        <f t="shared" si="2"/>
+        <v>11.987323494929036</v>
+      </c>
+      <c r="U41" s="16">
+        <v>1</v>
+      </c>
+      <c r="V41" s="17">
+        <f t="shared" si="3"/>
+        <v>3.7050059654208249</v>
       </c>
     </row>
-    <row r="39" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O39" s="9">
-        <v>32</v>
-      </c>
-      <c r="P39" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q39" s="9">
+    <row r="42" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P42" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999953433871</v>
-      </c>
-      <c r="R39" s="9">
-        <v>1</v>
-      </c>
-      <c r="S39" s="9">
-        <f>($I$16*S38)+($K$16*R36)+($L$16*R35)</f>
-        <v>3.7048548031019326</v>
+        <v>33</v>
+      </c>
+      <c r="Q42" s="30">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="R42" s="21">
+        <v>34</v>
+      </c>
+      <c r="S42" s="16">
+        <v>1</v>
+      </c>
+      <c r="T42" s="17">
+        <f t="shared" si="2"/>
+        <v>11.989858795663832</v>
+      </c>
+      <c r="U42" s="16">
+        <v>1</v>
+      </c>
+      <c r="V42" s="17">
+        <f t="shared" ref="V42:V73" si="4">($J$17*V41)+($L$17*U39)+($M$17*U38)</f>
+        <v>3.7051180162971891</v>
       </c>
     </row>
-    <row r="40" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O40" s="9">
-        <v>33</v>
-      </c>
-      <c r="P40" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q40" s="9">
+    <row r="43" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P43" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999976716936</v>
-      </c>
-      <c r="R40" s="9">
-        <v>1</v>
-      </c>
-      <c r="S40" s="9">
-        <f>($I$16*S39)+($K$16*R37)+($L$16*R36)</f>
-        <v>3.7050059654208249</v>
+        <v>34</v>
+      </c>
+      <c r="Q43" s="30">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="R43" s="21">
+        <v>35</v>
+      </c>
+      <c r="S43" s="16">
+        <v>1</v>
+      </c>
+      <c r="T43" s="17">
+        <f t="shared" si="2"/>
+        <v>11.991887036391367</v>
+      </c>
+      <c r="U43" s="16">
+        <v>1</v>
+      </c>
+      <c r="V43" s="17">
+        <f t="shared" si="4"/>
+        <v>3.7052010753491142</v>
       </c>
     </row>
-    <row r="41" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O41" s="9">
-        <v>34</v>
-      </c>
-      <c r="P41" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q41" s="9">
+    <row r="44" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P44" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999988358468</v>
-      </c>
-      <c r="R41" s="9">
-        <v>1</v>
-      </c>
-      <c r="S41" s="9">
-        <f>($I$16*S40)+($K$16*R38)+($L$16*R37)</f>
-        <v>3.7051180162971891</v>
+        <v>35</v>
+      </c>
+      <c r="Q44" s="30">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="R44" s="21">
+        <v>36</v>
+      </c>
+      <c r="S44" s="16">
+        <v>1</v>
+      </c>
+      <c r="T44" s="17">
+        <f t="shared" si="2"/>
+        <v>11.993509629043244</v>
+      </c>
+      <c r="U44" s="16">
+        <v>1</v>
+      </c>
+      <c r="V44" s="17">
+        <f t="shared" si="4"/>
+        <v>3.7052626438645113</v>
       </c>
     </row>
-    <row r="42" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O42" s="9">
-        <v>35</v>
-      </c>
-      <c r="P42" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q42" s="9">
+    <row r="45" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P45" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999994179234</v>
-      </c>
-      <c r="R42" s="9">
-        <v>1</v>
-      </c>
-      <c r="S42" s="9">
-        <f>($I$16*S41)+($K$16*R39)+($L$16*R38)</f>
-        <v>3.7052010753491142</v>
+        <v>36</v>
+      </c>
+      <c r="Q45" s="30">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="R45" s="21">
+        <v>37</v>
+      </c>
+      <c r="S45" s="16">
+        <v>1</v>
+      </c>
+      <c r="T45" s="17">
+        <f t="shared" si="2"/>
+        <v>11.994807703199671</v>
+      </c>
+      <c r="U45" s="16">
+        <v>1</v>
+      </c>
+      <c r="V45" s="17">
+        <f t="shared" si="4"/>
+        <v>3.7053082822627399</v>
       </c>
     </row>
-    <row r="43" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O43" s="9">
-        <v>36</v>
-      </c>
-      <c r="P43" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q43" s="9">
+    <row r="46" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P46" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999997089617</v>
-      </c>
-      <c r="R43" s="9">
-        <v>1</v>
-      </c>
-      <c r="S43" s="9">
-        <f>($I$16*S42)+($K$16*R40)+($L$16*R39)</f>
-        <v>3.7052626438645113</v>
+        <v>37</v>
+      </c>
+      <c r="Q46" s="30">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="R46" s="21">
+        <v>38</v>
+      </c>
+      <c r="S46" s="16">
+        <v>1</v>
+      </c>
+      <c r="T46" s="17">
+        <f t="shared" si="2"/>
+        <v>11.995846162542275</v>
+      </c>
+      <c r="U46" s="16">
+        <v>1</v>
+      </c>
+      <c r="V46" s="17">
+        <f t="shared" si="4"/>
+        <v>3.7053421122711363</v>
       </c>
     </row>
-    <row r="44" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O44" s="9">
-        <v>37</v>
-      </c>
-      <c r="P44" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q44" s="9">
+    <row r="47" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P47" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999998544808</v>
-      </c>
-      <c r="R44" s="9">
-        <v>1</v>
-      </c>
-      <c r="S44" s="9">
-        <f>($I$16*S43)+($K$16*R41)+($L$16*R40)</f>
-        <v>3.7053082822627399</v>
+        <v>38</v>
+      </c>
+      <c r="Q47" s="30">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="R47" s="21">
+        <v>39</v>
+      </c>
+      <c r="S47" s="16">
+        <v>1</v>
+      </c>
+      <c r="T47" s="17">
+        <f t="shared" si="2"/>
+        <v>11.996676930025089</v>
+      </c>
+      <c r="U47" s="16">
+        <v>1</v>
+      </c>
+      <c r="V47" s="17">
+        <f t="shared" si="4"/>
+        <v>3.7053671891693742</v>
       </c>
     </row>
-    <row r="45" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O45" s="9">
-        <v>38</v>
-      </c>
-      <c r="P45" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q45" s="9">
+    <row r="48" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P48" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999999272404</v>
-      </c>
-      <c r="R45" s="9">
-        <v>1</v>
-      </c>
-      <c r="S45" s="9">
-        <f>($I$16*S44)+($K$16*R42)+($L$16*R41)</f>
-        <v>3.7053421122711363</v>
+        <v>39</v>
+      </c>
+      <c r="Q48" s="30">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="R48" s="21">
+        <v>40</v>
+      </c>
+      <c r="S48" s="16">
+        <v>1</v>
+      </c>
+      <c r="T48" s="17">
+        <f t="shared" si="2"/>
+        <v>11.997341544015704</v>
+      </c>
+      <c r="U48" s="16">
+        <v>1</v>
+      </c>
+      <c r="V48" s="17">
+        <f t="shared" si="4"/>
+        <v>3.7053857777200436</v>
       </c>
     </row>
-    <row r="46" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O46" s="9">
-        <v>39</v>
-      </c>
-      <c r="P46" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q46" s="9">
+    <row r="49" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P49" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999999636202</v>
-      </c>
-      <c r="R46" s="9">
-        <v>1</v>
-      </c>
-      <c r="S46" s="9">
-        <f>($I$16*S45)+($K$16*R43)+($L$16*R42)</f>
-        <v>3.7053671891693742</v>
+        <v>40</v>
+      </c>
+      <c r="Q49" s="30">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="R49" s="21">
+        <v>41</v>
+      </c>
+      <c r="S49" s="16">
+        <v>1</v>
+      </c>
+      <c r="T49" s="17">
+        <f t="shared" si="2"/>
+        <v>11.997873235210379</v>
+      </c>
+      <c r="U49" s="16">
+        <v>1</v>
+      </c>
+      <c r="V49" s="17">
+        <f t="shared" si="4"/>
+        <v>3.7053995567054949</v>
       </c>
     </row>
-    <row r="47" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O47" s="9">
-        <v>40</v>
-      </c>
-      <c r="P47" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q47" s="9">
+    <row r="50" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P50" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999999818101</v>
-      </c>
-      <c r="R47" s="9">
-        <v>1</v>
-      </c>
-      <c r="S47" s="9">
-        <f>($I$16*S46)+($K$16*R44)+($L$16*R43)</f>
-        <v>3.7053857777200436</v>
+        <v>41</v>
+      </c>
+      <c r="Q50" s="30">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="R50" s="21">
+        <v>42</v>
+      </c>
+      <c r="S50" s="16">
+        <v>1</v>
+      </c>
+      <c r="T50" s="17">
+        <f t="shared" si="2"/>
+        <v>11.998298588167211</v>
+      </c>
+      <c r="U50" s="16">
+        <v>1</v>
+      </c>
+      <c r="V50" s="17">
+        <f t="shared" si="4"/>
+        <v>3.7054097705432198</v>
       </c>
     </row>
-    <row r="48" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O48" s="9">
-        <v>41</v>
-      </c>
-      <c r="P48" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q48" s="9">
+    <row r="51" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P51" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999999909051</v>
-      </c>
-      <c r="R48" s="9">
-        <v>1</v>
-      </c>
-      <c r="S48" s="9">
-        <f>($I$16*S47)+($K$16*R45)+($L$16*R44)</f>
-        <v>3.7053995567054949</v>
+        <v>42</v>
+      </c>
+      <c r="Q51" s="30">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="R51" s="21">
+        <v>43</v>
+      </c>
+      <c r="S51" s="16">
+        <v>1</v>
+      </c>
+      <c r="T51" s="17">
+        <f t="shared" si="2"/>
+        <v>11.998638870533222</v>
+      </c>
+      <c r="U51" s="16">
+        <v>1</v>
+      </c>
+      <c r="V51" s="17">
+        <f t="shared" si="4"/>
+        <v>3.7054173416725629</v>
       </c>
     </row>
-    <row r="49" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O49" s="9">
-        <v>42</v>
-      </c>
-      <c r="P49" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q49" s="9">
+    <row r="52" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P52" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999999954525</v>
-      </c>
-      <c r="R49" s="9">
-        <v>1</v>
-      </c>
-      <c r="S49" s="9">
-        <f>($I$16*S48)+($K$16*R46)+($L$16*R45)</f>
-        <v>3.7054097705432198</v>
+        <v>43</v>
+      </c>
+      <c r="Q52" s="30">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="R52" s="21">
+        <v>44</v>
+      </c>
+      <c r="S52" s="16">
+        <v>1</v>
+      </c>
+      <c r="T52" s="17">
+        <f t="shared" si="2"/>
+        <v>11.998911096426305</v>
+      </c>
+      <c r="U52" s="16">
+        <v>1</v>
+      </c>
+      <c r="V52" s="17">
+        <f t="shared" si="4"/>
+        <v>3.7054229538627181</v>
       </c>
     </row>
-    <row r="50" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O50" s="9">
-        <v>43</v>
-      </c>
-      <c r="P50" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q50" s="9">
+    <row r="53" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P53" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999999977263</v>
-      </c>
-      <c r="R50" s="9">
-        <v>1</v>
-      </c>
-      <c r="S50" s="9">
-        <f>($I$16*S49)+($K$16*R47)+($L$16*R46)</f>
-        <v>3.7054173416725629</v>
+        <v>44</v>
+      </c>
+      <c r="Q53" s="30">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="R53" s="21">
+        <v>45</v>
+      </c>
+      <c r="S53" s="16">
+        <v>1</v>
+      </c>
+      <c r="T53" s="17">
+        <f t="shared" si="2"/>
+        <v>11.999128877140908</v>
+      </c>
+      <c r="U53" s="16">
+        <v>1</v>
+      </c>
+      <c r="V53" s="17">
+        <f t="shared" si="4"/>
+        <v>3.7054271139657766</v>
       </c>
     </row>
-    <row r="51" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O51" s="9">
-        <v>44</v>
-      </c>
-      <c r="P51" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q51" s="9">
+    <row r="54" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P54" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999999988631</v>
-      </c>
-      <c r="R51" s="9">
-        <v>1</v>
-      </c>
-      <c r="S51" s="9">
-        <f>($I$16*S50)+($K$16*R48)+($L$16*R47)</f>
-        <v>3.7054229538627181</v>
+        <v>45</v>
+      </c>
+      <c r="Q54" s="30">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="R54" s="21">
+        <v>46</v>
+      </c>
+      <c r="S54" s="16">
+        <v>1</v>
+      </c>
+      <c r="T54" s="17">
+        <f t="shared" si="2"/>
+        <v>11.999303101712657</v>
+      </c>
+      <c r="U54" s="16">
+        <v>1</v>
+      </c>
+      <c r="V54" s="17">
+        <f t="shared" si="4"/>
+        <v>3.7054301976919124</v>
       </c>
     </row>
-    <row r="52" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O52" s="9">
-        <v>45</v>
-      </c>
-      <c r="P52" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q52" s="9">
+    <row r="55" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P55" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999999994316</v>
-      </c>
-      <c r="R52" s="9">
-        <v>1</v>
-      </c>
-      <c r="S52" s="9">
-        <f>($I$16*S51)+($K$16*R49)+($L$16*R48)</f>
-        <v>3.7054271139657766</v>
+        <v>46</v>
+      </c>
+      <c r="Q55" s="30">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="R55" s="21">
+        <v>47</v>
+      </c>
+      <c r="S55" s="16">
+        <v>1</v>
+      </c>
+      <c r="T55" s="17">
+        <f t="shared" si="2"/>
+        <v>11.999442481370091</v>
+      </c>
+      <c r="U55" s="16">
+        <v>1</v>
+      </c>
+      <c r="V55" s="17">
+        <f t="shared" si="4"/>
+        <v>3.7054324835407835</v>
       </c>
     </row>
-    <row r="53" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O53" s="9">
-        <v>46</v>
-      </c>
-      <c r="P53" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q53" s="9">
+    <row r="56" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P56" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999999997158</v>
-      </c>
-      <c r="R53" s="9">
-        <v>1</v>
-      </c>
-      <c r="S53" s="9">
-        <f>($I$16*S52)+($K$16*R50)+($L$16*R49)</f>
-        <v>3.7054301976919124</v>
+        <v>47</v>
+      </c>
+      <c r="Q56" s="30">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="R56" s="21">
+        <v>48</v>
+      </c>
+      <c r="S56" s="16">
+        <v>1</v>
+      </c>
+      <c r="T56" s="17">
+        <f t="shared" si="2"/>
+        <v>11.999553985096055</v>
+      </c>
+      <c r="U56" s="16">
+        <v>1</v>
+      </c>
+      <c r="V56" s="17">
+        <f t="shared" si="4"/>
+        <v>3.7054341779535918</v>
       </c>
     </row>
-    <row r="54" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O54" s="9">
-        <v>47</v>
-      </c>
-      <c r="P54" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q54" s="9">
+    <row r="57" spans="16:22" x14ac:dyDescent="0.2">
+      <c r="P57" s="33">
         <f t="shared" si="0"/>
-        <v>0.99999999999998579</v>
-      </c>
-      <c r="R54" s="9">
-        <v>1</v>
-      </c>
-      <c r="S54" s="9">
-        <f>($I$16*S53)+($K$16*R51)+($L$16*R50)</f>
-        <v>3.7054324835407835</v>
+        <v>48</v>
+      </c>
+      <c r="Q57" s="30">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="R57" s="21">
+        <v>49</v>
+      </c>
+      <c r="S57" s="16">
+        <v>1</v>
+      </c>
+      <c r="T57" s="17">
+        <f t="shared" si="2"/>
+        <v>11.999643188076835</v>
+      </c>
+      <c r="U57" s="16">
+        <v>1</v>
+      </c>
+      <c r="V57" s="17">
+        <f t="shared" si="4"/>
+        <v>3.7054354339573461</v>
       </c>
     </row>
-    <row r="55" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O55" s="9">
-        <v>48</v>
-      </c>
-      <c r="P55" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q55" s="9">
+    <row r="58" spans="16:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P58" s="40">
         <f t="shared" si="0"/>
-        <v>0.99999999999999289</v>
-      </c>
-      <c r="R55" s="9">
-        <v>1</v>
-      </c>
-      <c r="S55" s="9">
-        <f>($I$16*S54)+($K$16*R52)+($L$16*R51)</f>
-        <v>3.7054341779535918</v>
-      </c>
-    </row>
-    <row r="56" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O56" s="9">
         <v>49</v>
       </c>
-      <c r="P56" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q56" s="9">
-        <f t="shared" si="0"/>
-        <v>0.99999999999999645</v>
-      </c>
-      <c r="R56" s="9">
-        <v>1</v>
-      </c>
-      <c r="S56" s="9">
-        <f>($I$16*S55)+($K$16*R53)+($L$16*R52)</f>
-        <v>3.7054354339573461</v>
-      </c>
-    </row>
-    <row r="57" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O57" s="9">
+      <c r="Q58" s="41">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="R58" s="22">
         <v>50</v>
       </c>
-      <c r="P57" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q57" s="9">
-        <f t="shared" si="0"/>
-        <v>0.99999999999999822</v>
-      </c>
-      <c r="R57" s="9">
-        <v>1</v>
-      </c>
-      <c r="S57" s="9">
-        <f>($I$16*S56)+($K$16*R54)+($L$16*R53)</f>
+      <c r="S58" s="18">
+        <v>1</v>
+      </c>
+      <c r="T58" s="17">
+        <f t="shared" si="2"/>
+        <v>11.999714550461462</v>
+      </c>
+      <c r="U58" s="18">
+        <v>1</v>
+      </c>
+      <c r="V58" s="19">
+        <f t="shared" si="4"/>
         <v>3.7054363649851476</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="I14:M14"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="I8:J8"/>
+  <mergeCells count="9">
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>